<commit_message>
118 Add Explore System
</commit_message>
<xml_diff>
--- a/GameMaster/GameDesign/GamePlay.xlsx
+++ b/GameMaster/GameDesign/GamePlay.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\建造工程\Project\GameMaster\GameDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC20954F-A098-4198-BC70-A1441943DFAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC963E7-FD3C-47D1-BA63-9606FB6C7BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2100" yWindow="1110" windowWidth="26295" windowHeight="13635" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16200" yWindow="3735" windowWidth="26295" windowHeight="13635" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="空" sheetId="9" r:id="rId1"/>
     <sheet name="背景" sheetId="1" r:id="rId2"/>
     <sheet name="科技树" sheetId="14" r:id="rId3"/>
     <sheet name="GamePlay" sheetId="3" r:id="rId4"/>
-    <sheet name="机械组装" sheetId="12" r:id="rId5"/>
-    <sheet name="建筑" sheetId="5" r:id="rId6"/>
-    <sheet name="战斗" sheetId="10" r:id="rId7"/>
-    <sheet name="订单" sheetId="7" r:id="rId8"/>
-    <sheet name="Ref" sheetId="2" r:id="rId9"/>
+    <sheet name="探索" sheetId="15" r:id="rId5"/>
+    <sheet name="机械组装" sheetId="12" r:id="rId6"/>
+    <sheet name="建筑" sheetId="5" r:id="rId7"/>
+    <sheet name="战斗" sheetId="10" r:id="rId8"/>
+    <sheet name="订单" sheetId="7" r:id="rId9"/>
+    <sheet name="Ref" sheetId="2" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="378">
   <si>
     <t>概述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1413,6 +1414,114 @@
   </si>
   <si>
     <t>虹石（资金）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>探索</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>探索准备：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>探索过程：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>探索路线选择（选择探索点）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个探索点拥有不同消耗值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>起始点——某个分支——具体点位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>路线选择：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>探索奖励/惩罚：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>丢失物品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得物品</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>失去人员</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获得科技加成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 选择目标点：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>决定后续事件基础</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 探索队配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人员配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>燃料</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主要资源配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点位分支剧情选择</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>探索结果（最终）：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>资源携带上限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单次探索配置携带上限</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类似galgame，会开启一个局内事件串，导向不同结果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>属性：</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>探索难度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>探索大区——大区分支（按完成度随机）——具体单次探索分支生成——探索点</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1420,7 +1529,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1518,6 +1627,15 @@
       <name val="微软雅黑"/>
       <family val="2"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1650,7 +1768,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1692,6 +1810,7 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1915,6 +2034,99 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>13158</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C8F7EBE-3DFC-4368-A8AA-33DD75271A7A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9944100" y="838200"/>
+          <a:ext cx="3099258" cy="3105150"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>180513</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F414A0FC-5EC2-49E0-B617-7D36A0EE2092}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13373100" y="838200"/>
+          <a:ext cx="4800600" cy="3076113"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2156,7 +2368,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2205,7 +2417,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -3064,11 +3276,30 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C308F5-7B8D-4001-80FC-1B7282245A29}">
+  <dimension ref="A1:U1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="21" width="9" style="1"/>
+  </cols>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AN143"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
+    <sheetView topLeftCell="A88" workbookViewId="0">
       <selection activeCell="P71" sqref="P71"/>
     </sheetView>
   </sheetViews>
@@ -4913,8 +5144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0120ED9E-5CAF-4371-8D30-5A3CFD184EC2}">
   <dimension ref="A2:AS70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R57" sqref="R57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5177,11 +5408,281 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09797122-A2D1-404C-B60F-D9A4B10EDD62}">
+  <dimension ref="A1:BT41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AS6" sqref="AS6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="50" width="4.5" style="1" customWidth="1"/>
+    <col min="51" max="72" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:72" s="37" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="38" t="s">
+        <v>351</v>
+      </c>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+    </row>
+    <row r="3" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="B3" s="39" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="5" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="C5" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="7" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="B7" s="39" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="8" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="B8" s="39"/>
+    </row>
+    <row r="9" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="B9" s="39"/>
+      <c r="C9" s="39" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="B10" s="39"/>
+      <c r="D10" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="11" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="B11" s="39"/>
+      <c r="D11" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="12" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="B12" s="39"/>
+    </row>
+    <row r="13" spans="1:72" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="26"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="26"/>
+      <c r="K13" s="26"/>
+      <c r="L13" s="26"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="26"/>
+      <c r="W13" s="26"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
+      <c r="AA13" s="26"/>
+      <c r="AB13" s="26"/>
+      <c r="AC13" s="26"/>
+      <c r="AD13" s="26"/>
+      <c r="AE13" s="26"/>
+      <c r="AF13" s="26"/>
+      <c r="AG13" s="26"/>
+      <c r="AH13" s="26"/>
+      <c r="AI13" s="26"/>
+      <c r="AJ13" s="26"/>
+      <c r="AK13" s="26"/>
+      <c r="AL13" s="26"/>
+      <c r="AM13" s="26"/>
+      <c r="AN13" s="26"/>
+      <c r="AO13" s="26"/>
+      <c r="AP13" s="26"/>
+      <c r="AQ13" s="26"/>
+      <c r="AR13" s="26"/>
+      <c r="AS13" s="26"/>
+      <c r="AT13" s="26"/>
+      <c r="AU13" s="26"/>
+      <c r="AV13" s="26"/>
+      <c r="AW13" s="26"/>
+      <c r="AX13" s="26"/>
+      <c r="AY13" s="26"/>
+      <c r="AZ13" s="26"/>
+      <c r="BA13" s="26"/>
+      <c r="BB13" s="26"/>
+      <c r="BC13" s="26"/>
+      <c r="BD13" s="26"/>
+      <c r="BE13" s="26"/>
+      <c r="BF13" s="26"/>
+      <c r="BG13" s="26"/>
+      <c r="BH13" s="26"/>
+      <c r="BI13" s="26"/>
+      <c r="BJ13" s="26"/>
+      <c r="BK13" s="26"/>
+      <c r="BL13" s="26"/>
+      <c r="BM13" s="26"/>
+      <c r="BN13" s="26"/>
+      <c r="BO13" s="26"/>
+      <c r="BP13" s="26"/>
+      <c r="BQ13" s="26"/>
+      <c r="BR13" s="26"/>
+      <c r="BS13" s="26"/>
+      <c r="BT13" s="26"/>
+    </row>
+    <row r="14" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="C14" s="1" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="15" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="D15" s="1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C17" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D18" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D19" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D21" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E22" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B24" s="39" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C25" s="39" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C26" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C27" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C29" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C31" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="D32" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B35" s="39" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C37" s="39" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C38" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C39" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C40" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C41" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FF3815B-1C64-4706-B37F-583C253BF8E3}">
   <dimension ref="A1:AN80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -5899,7 +6400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E27657-09A1-4075-9543-85D2D8132F35}">
   <dimension ref="A2:AN58"/>
   <sheetViews>
@@ -6642,7 +7143,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D3B62E0-DBD4-4041-9B0F-16875A209E23}">
   <dimension ref="A2:AN135"/>
   <sheetViews>
@@ -7896,7 +8397,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF733293-B9C4-4FA9-8647-0B1ABC272B09}">
   <dimension ref="A2:AN89"/>
   <sheetViews>
@@ -8729,23 +9230,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C308F5-7B8D-4001-80FC-1B7282245A29}">
-  <dimension ref="A1:U1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="21" width="9" style="1"/>
-  </cols>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
121 Add Explore Resources
</commit_message>
<xml_diff>
--- a/GameMaster/GameDesign/GamePlay.xlsx
+++ b/GameMaster/GameDesign/GamePlay.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\建造工程\Project\GameMaster\GameDesign\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC963E7-FD3C-47D1-BA63-9606FB6C7BC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A9D1D90-C26F-4840-B10C-FB2151C72AE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16200" yWindow="3735" windowWidth="26295" windowHeight="13635" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3360" yWindow="2145" windowWidth="24780" windowHeight="12330" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="空" sheetId="9" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="382">
   <si>
     <t>概述</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1522,6 +1522,22 @@
   </si>
   <si>
     <t>探索大区——大区分支（按完成度随机）——具体单次探索分支生成——探索点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工具人，只配置类型与数量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人员限制‘’</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞船限制、等级限制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>飞船配置</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2039,13 +2055,13 @@
     <xdr:from>
       <xdr:col>29</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>13158</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2083,13 +2099,13 @@
     <xdr:from>
       <xdr:col>39</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>51</xdr:col>
       <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>180513</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5409,10 +5425,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09797122-A2D1-404C-B60F-D9A4B10EDD62}">
-  <dimension ref="A1:BT41"/>
+  <dimension ref="A1:BT42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AS6" sqref="AS6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5494,12 +5510,17 @@
     </row>
     <row r="12" spans="1:72" x14ac:dyDescent="0.2">
       <c r="B12" s="39"/>
+      <c r="D12" s="1" t="s">
+        <v>379</v>
+      </c>
     </row>
     <row r="13" spans="1:72" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26"/>
       <c r="B13" s="26"/>
       <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="D13" s="26" t="s">
+        <v>380</v>
+      </c>
       <c r="E13" s="26"/>
       <c r="F13" s="26"/>
       <c r="G13" s="26"/>
@@ -5569,103 +5590,185 @@
       <c r="BS13" s="26"/>
       <c r="BT13" s="26"/>
     </row>
-    <row r="14" spans="1:72" x14ac:dyDescent="0.2">
-      <c r="C14" s="1" t="s">
+    <row r="14" spans="1:72" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="26"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="J14" s="26"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="26"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
+      <c r="W14" s="26"/>
+      <c r="X14" s="26"/>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
+      <c r="AA14" s="26"/>
+      <c r="AB14" s="26"/>
+      <c r="AC14" s="26"/>
+      <c r="AD14" s="26"/>
+      <c r="AE14" s="26"/>
+      <c r="AF14" s="26"/>
+      <c r="AG14" s="26"/>
+      <c r="AH14" s="26"/>
+      <c r="AI14" s="26"/>
+      <c r="AJ14" s="26"/>
+      <c r="AK14" s="26"/>
+      <c r="AL14" s="26"/>
+      <c r="AM14" s="26"/>
+      <c r="AN14" s="26"/>
+      <c r="AO14" s="26"/>
+      <c r="AP14" s="26"/>
+      <c r="AQ14" s="26"/>
+      <c r="AR14" s="26"/>
+      <c r="AS14" s="26"/>
+      <c r="AT14" s="26"/>
+      <c r="AU14" s="26"/>
+      <c r="AV14" s="26"/>
+      <c r="AW14" s="26"/>
+      <c r="AX14" s="26"/>
+      <c r="AY14" s="26"/>
+      <c r="AZ14" s="26"/>
+      <c r="BA14" s="26"/>
+      <c r="BB14" s="26"/>
+      <c r="BC14" s="26"/>
+      <c r="BD14" s="26"/>
+      <c r="BE14" s="26"/>
+      <c r="BF14" s="26"/>
+      <c r="BG14" s="26"/>
+      <c r="BH14" s="26"/>
+      <c r="BI14" s="26"/>
+      <c r="BJ14" s="26"/>
+      <c r="BK14" s="26"/>
+      <c r="BL14" s="26"/>
+      <c r="BM14" s="26"/>
+      <c r="BN14" s="26"/>
+      <c r="BO14" s="26"/>
+      <c r="BP14" s="26"/>
+      <c r="BQ14" s="26"/>
+      <c r="BR14" s="26"/>
+      <c r="BS14" s="26"/>
+      <c r="BT14" s="26"/>
+    </row>
+    <row r="15" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="C15" s="1" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="15" spans="1:72" x14ac:dyDescent="0.2">
-      <c r="D15" s="1" t="s">
+    <row r="16" spans="1:72" x14ac:dyDescent="0.2">
+      <c r="D16" s="1" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C17" s="1" t="s">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C18" s="1" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D18" s="1" t="s">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D19" s="1" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D19" s="1" t="s">
+      <c r="G19" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D20" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="D21" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="D22" s="1" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E22" s="1" t="s">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="E23" s="1" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B24" s="39" t="s">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="39" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C25" s="39" t="s">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C26" s="39" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C26" s="1" t="s">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C27" s="1" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C27" s="1" t="s">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C28" s="1" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C29" s="1" t="s">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C30" s="1" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="C31" s="1" t="s">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="C32" s="1" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="D32" s="1" t="s">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="1" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B35" s="39" t="s">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="39" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C37" s="39" t="s">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C38" s="39" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C38" s="1" t="s">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C39" s="1" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C39" s="1" t="s">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C40" s="1" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C40" s="1" t="s">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C41" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C41" s="1" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C42" s="1" t="s">
         <v>362</v>
       </c>
     </row>

</xml_diff>